<commit_message>
Updated Delete_File class functionality, more testing done with these changes Updated Create_File class functionality, tested added javadoc to all package files
</commit_message>
<xml_diff>
--- a/app/src/test/java/FileManagment/Delete_File.xlsx
+++ b/app/src/test/java/FileManagment/Delete_File.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\Documents\Uni 2018\Sem 2\Capstone\Testing\File Creation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Patrick\Documents\Uni 2018\Sem 2\Capstone\Android App\2018-02-healthcare-visualization-data-tracking-application\app\src\test\java\FileManagment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02A07DF3-4FED-48D6-B347-129F338FB60B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98479776-98E0-4426-8C32-A7E6E9C2A754}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12165" xr2:uid="{A330BECD-E836-4AC6-938E-7E613B009CCC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7680" xr2:uid="{A330BECD-E836-4AC6-938E-7E613B009CCC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="54">
   <si>
     <t>Step Number</t>
   </si>
@@ -84,27 +84,15 @@
     <t>Invalid Task</t>
   </si>
   <si>
-    <t>file, Delete_Account_File, "test"</t>
-  </si>
-  <si>
     <t>Invalid_Task_Exception</t>
   </si>
   <si>
     <t>File_Exception</t>
   </si>
   <si>
-    <t>Test Name:Delete File Test</t>
-  </si>
-  <si>
-    <t>Delete File Test</t>
-  </si>
-  <si>
     <t>Purpose: Test the Unit Logic of the Delete_File Class</t>
   </si>
   <si>
-    <t>Comments: The private inner files that deal with file deletion aren’t tested due to the requirment System IO commands requiring the OS. Mockito was used to mock the injected File Object to trigger outputs</t>
-  </si>
-  <si>
     <t>Assumptions/Dependencies: The File Deletion will be tested during intergration with the android system</t>
   </si>
   <si>
@@ -117,22 +105,88 @@
     <t>file, Delete_Review_File, null</t>
   </si>
   <si>
-    <t>file, Delete_Account, "test"</t>
-  </si>
-  <si>
-    <t>file, Delete_Medical_File, "test"</t>
-  </si>
-  <si>
-    <t>Cant_del_NewReviewFile</t>
-  </si>
-  <si>
-    <t>Cant_del_NewMedicalFile</t>
-  </si>
-  <si>
-    <t>Cant_del_NewAccountFile</t>
-  </si>
-  <si>
-    <t>Cant_del_NewAccountDir</t>
+    <t>Delete File Test v2</t>
+  </si>
+  <si>
+    <t>Test Name:Delete File Test v2</t>
+  </si>
+  <si>
+    <t>Del_AccountDir_Invalid_Name</t>
+  </si>
+  <si>
+    <t>Del_AccountDir_Fail</t>
+  </si>
+  <si>
+    <t>Del_AccountDir</t>
+  </si>
+  <si>
+    <t>Delete_Review_File_Invalid_Name</t>
+  </si>
+  <si>
+    <t>Delete_Review_File_Fail</t>
+  </si>
+  <si>
+    <t>Delete_Review_File</t>
+  </si>
+  <si>
+    <t>Delete_Account_File_Invalid_Name</t>
+  </si>
+  <si>
+    <t>Delete_Account_File_Fail</t>
+  </si>
+  <si>
+    <t>Delete_Account_File</t>
+  </si>
+  <si>
+    <t>Delete_Medical_File_Invalid_Name</t>
+  </si>
+  <si>
+    <t>Delete_Medical_File_Fail</t>
+  </si>
+  <si>
+    <t>Delete_Medical_File</t>
+  </si>
+  <si>
+    <t>Comments: The private inner files that deal with file deletion aren’t tested due to the requirment System IO commands requiring the OS. Mockito was used to mock the injected File Object to trigger and simulate functionality/problems</t>
+  </si>
+  <si>
+    <t>file, Delete_Review_File, "default"</t>
+  </si>
+  <si>
+    <t>file, Delete_Account_File, "default"</t>
+  </si>
+  <si>
+    <t>file, Delete_Medical_File, "bob"</t>
+  </si>
+  <si>
+    <t>not exceptions thrown</t>
+  </si>
+  <si>
+    <t>file, Delete_Account(name  = bob), "Fred"</t>
+  </si>
+  <si>
+    <t>file, Delete_Review_File(name = invalid), "default"</t>
+  </si>
+  <si>
+    <t>file, Delete_Medical_File(name = invalid), "default"</t>
+  </si>
+  <si>
+    <t>file, Delete_Account_File(delete() = false), "bob"</t>
+  </si>
+  <si>
+    <t>file, Delete_Account_File,(delete() = false) "default"</t>
+  </si>
+  <si>
+    <t>file, Delete_Medical_File,(delete() = false) "default"</t>
+  </si>
+  <si>
+    <t>file, Delete_Review_File(delete() = false), "default"</t>
+  </si>
+  <si>
+    <t>file, Delete_Account_File(name = invalid), "default"</t>
+  </si>
+  <si>
+    <t>file, Delete_Medicalt_File, "default"</t>
   </si>
 </sst>
 </file>
@@ -241,7 +295,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -253,6 +307,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -271,10 +331,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -591,7 +648,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3386EA7-E985-4B0C-876A-4522744B2EB5}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C18" sqref="C18"/>
@@ -605,69 +662,69 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
+      <c r="A1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
+      <c r="A2" s="8"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
     </row>
     <row r="3" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="12"/>
+    </row>
+    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A4" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="12"/>
+    </row>
+    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.35">
+      <c r="A5" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+    </row>
+    <row r="6" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" s="10"/>
-    </row>
-    <row r="4" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A4" s="10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" s="10"/>
-    </row>
-    <row r="5" spans="1:5" ht="21" x14ac:dyDescent="0.35">
-      <c r="A5" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B5" s="10"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-    </row>
-    <row r="6" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-    </row>
-    <row r="7" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="8"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="9"/>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
+    </row>
+    <row r="7" spans="1:5" ht="43.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="10"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="11"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
@@ -694,9 +751,9 @@
         <v>8</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E9" s="4" t="s">
@@ -713,7 +770,7 @@
       <c r="C10" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E10" s="4" t="s">
@@ -728,9 +785,9 @@
         <v>13</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D11" s="11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" s="5" t="s">
         <v>9</v>
       </c>
       <c r="E11" s="4" t="s">
@@ -745,9 +802,9 @@
         <v>14</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D12" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="5" t="s">
         <v>16</v>
       </c>
       <c r="E12" s="4" t="s">
@@ -762,9 +819,9 @@
         <v>17</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>16</v>
       </c>
       <c r="E13" s="4" t="s">
@@ -781,87 +838,216 @@
       <c r="C14" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>7</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="4" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A15" s="12">
-        <v>7</v>
-      </c>
-      <c r="B15" s="12" t="s">
+      <c r="E15" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A16" s="6">
+        <v>8</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" s="6">
+        <v>9</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="6">
+        <v>10</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>11</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" s="13">
+        <v>12</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="13">
+        <v>13</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="13">
+        <v>14</v>
+      </c>
+      <c r="B22" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="C15" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A16" s="12">
-        <v>8</v>
-      </c>
-      <c r="B16" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E16" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="12">
-        <v>9</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="12">
-        <v>10</v>
-      </c>
-      <c r="B18" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E18" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="3"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
+      <c r="C22" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" s="13">
+        <v>15</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="D23" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="13">
+        <v>16</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="13">
+        <v>17</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" s="13">
+        <v>18</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="D26" s="4" t="b">
+        <v>1</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>44</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>